<commit_message>
Created Visual Analysis to Consider Chart Exports, adjusted other functions
</commit_message>
<xml_diff>
--- a/ML - TCC - Clusters/tcc_ml_analysis/exploratory_analysis.xlsx
+++ b/ML - TCC - Clusters/tcc_ml_analysis/exploratory_analysis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>age</t>
   </si>
@@ -31,6 +31,9 @@
     <t>chol</t>
   </si>
   <si>
+    <t>thalach</t>
+  </si>
+  <si>
     <t>count</t>
   </si>
   <si>
@@ -64,9 +67,6 @@
     <t>restecg</t>
   </si>
   <si>
-    <t>thalach</t>
-  </si>
-  <si>
     <t>exang</t>
   </si>
   <si>
@@ -100,43 +100,43 @@
     <t>Sick</t>
   </si>
   <si>
-    <t>0.182</t>
-  </si>
-  <si>
-    <t>0.147</t>
-  </si>
-  <si>
-    <t>0.597</t>
+    <t>0.189</t>
+  </si>
+  <si>
+    <t>0.144</t>
+  </si>
+  <si>
+    <t>0.593</t>
   </si>
   <si>
     <t>0.03</t>
   </si>
   <si>
-    <t>0.085</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>0.069</t>
-  </si>
-  <si>
-    <t>0.44</t>
-  </si>
-  <si>
-    <t>0.358</t>
-  </si>
-  <si>
-    <t>0.425</t>
-  </si>
-  <si>
-    <t>0.323</t>
-  </si>
-  <si>
-    <t>0.476</t>
-  </si>
-  <si>
-    <t>0.617</t>
+    <t>0.086</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.067</t>
+  </si>
+  <si>
+    <t>0.388</t>
+  </si>
+  <si>
+    <t>0.356</t>
+  </si>
+  <si>
+    <t>0.422</t>
+  </si>
+  <si>
+    <t>0.319</t>
+  </si>
+  <si>
+    <t>0.474</t>
+  </si>
+  <si>
+    <t>0.614</t>
   </si>
   <si>
     <t>0.0</t>
@@ -497,13 +497,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,61 +516,73 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E2">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>301</v>
+      </c>
+      <c r="F2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>54.39735099337749</v>
+        <v>54.37873754152824</v>
       </c>
       <c r="C3">
-        <v>0.6821192052980133</v>
+        <v>0.6843853820598007</v>
       </c>
       <c r="D3">
-        <v>131.7450331125828</v>
+        <v>131.7840531561462</v>
       </c>
       <c r="E3">
-        <v>245.6423841059603</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>245.8671096345515</v>
+      </c>
+      <c r="F3">
+        <v>149.7508305647841</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>9.024572928814457</v>
+        <v>9.033792839530502</v>
       </c>
       <c r="C4">
-        <v>0.4664257380672638</v>
+        <v>0.4655341423056631</v>
       </c>
       <c r="D4">
-        <v>17.60260547288712</v>
+        <v>17.61883116205967</v>
       </c>
       <c r="E4">
-        <v>48.51959146323213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>48.44270445193932</v>
+      </c>
+      <c r="F4">
+        <v>22.73311184831199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>29</v>
@@ -584,10 +596,13 @@
       <c r="E5">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>48</v>
@@ -601,13 +616,16 @@
       <c r="E6">
         <v>211</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>55.5</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -616,12 +634,15 @@
         <v>130</v>
       </c>
       <c r="E7">
-        <v>240.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>241</v>
+      </c>
+      <c r="F7">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>61</v>
@@ -633,12 +654,15 @@
         <v>140</v>
       </c>
       <c r="E8">
-        <v>274.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>275</v>
+      </c>
+      <c r="F8">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>77</v>
@@ -651,6 +675,9 @@
       </c>
       <c r="E9">
         <v>417</v>
+      </c>
+      <c r="F9">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -674,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -683,13 +710,13 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
@@ -974,13 +1001,13 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -988,10 +1015,10 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>139</v>
@@ -1065,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1074,13 +1101,13 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>

</xml_diff>